<commit_message>
Wed, Aug 27 materials.
</commit_message>
<xml_diff>
--- a/fall25/math121/ClassDataFall25section05.xlsx
+++ b/fall25/math121/ClassDataFall25section05.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t xml:space="preserve">Height</t>
   </si>
@@ -268,7 +268,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,10 +540,18 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>

</xml_diff>